<commit_message>
working on tier 2 data
</commit_message>
<xml_diff>
--- a/data_prep/outputs/gday_data_assumptions_tier2.xlsx
+++ b/data_prep/outputs/gday_data_assumptions_tier2.xlsx
@@ -86,27 +86,18 @@
     <t>Chose 2017 GFDx estimate (172 g/day) over number from 2007 paper (162 g/day) that estimated from FAO balance sheets.</t>
   </si>
   <si>
-    <t>Chose 2019 GFDx number (33 g/gday) over 2000-2009 estimate of wheat (not specifically flour) (35 g/day) and over 1997-2000 survey estimate (17 g/day)</t>
-  </si>
-  <si>
     <t>Uganda</t>
   </si>
   <si>
     <t>https://fortificationdata.org/country-fortification-dashboard/?alpha3_code=UGA&amp;lang=en</t>
   </si>
   <si>
-    <t>Chose 2017 GFDx estimate (126 g/day) over number from 2007 paper (67 g/day) that estimated from FAO balance sheets, and a 1997-2000 report that estimated from FAO balance sheets</t>
-  </si>
-  <si>
     <t>g/day of wheat flour consumed (total population)</t>
   </si>
   <si>
     <t>Chose 2017 GFDx estimate (30 g/day) over number from 2000-2009 paper (24 g/day) that estimated wheat (not specifically wheat flour), and a 1997-2000 report that estimated (7 g/day) from FAO balance sheets</t>
   </si>
   <si>
-    <t>Chose 2017 GFDx estimte (283 g/day) over a 2007 paper that estimated (288 g/day) from FAO balance sheets and a 1997-2000 paper that estimated (204 g/day) from FAO balance sheets</t>
-  </si>
-  <si>
     <t>https://fortificationdata.org/country-fortification-dashboard/?alpha3_code=ZAF&amp;lang=en</t>
   </si>
   <si>
@@ -114,6 +105,15 @@
   </si>
   <si>
     <t>Chose 2017 GFDx estimate (156 g/day) over number from 2000-2009 paper (163 g/day) that estimated wheat (not specifically wheat flour), and a 1997-2000 report that estimated (123 g/day) from FAO balance sheets</t>
+  </si>
+  <si>
+    <t>Chose 2019 GFDx number (33 g/gday) over 2000-2009 estimate of wheat (not specifically flour) (35 g/day) and over 1997-2000 survey estimate (17 g/day).</t>
+  </si>
+  <si>
+    <t>Chose 2017 GFDx estimate (126 g/day) over number from 2007 paper (67 g/day) that estimated from FAO balance sheets, and a 1997-2000 report that estimated from FAO balance sheets.</t>
+  </si>
+  <si>
+    <t>Chose 2017 GFDx estimte (283 g/day) over a 2007 paper that estimated (288 g/day) from FAO balance sheets and a 1997-2000 paper that estimated (204 g/day) from FAO balance sheets.</t>
   </si>
 </sst>
 </file>
@@ -460,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44271</v>
       </c>
@@ -505,7 +505,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44271</v>
       </c>
@@ -539,7 +539,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44271</v>
       </c>
@@ -553,7 +553,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -561,16 +561,16 @@
         <v>44271</v>
       </c>
       <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -578,16 +578,16 @@
         <v>44271</v>
       </c>
       <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
       <c r="E7" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -595,16 +595,16 @@
         <v>44271</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -612,16 +612,16 @@
         <v>44271</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="390" x14ac:dyDescent="0.25">

</xml_diff>